<commit_message>
Add Music.csv and Music.xlsx files; update .gitignore to include Music.csv lock files
</commit_message>
<xml_diff>
--- a/necessary-items.xlsx
+++ b/necessary-items.xlsx
@@ -127,7 +127,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,6 +152,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,10 +176,10 @@
   <dimension ref="A1:XFD100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D100"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.47"/>
@@ -205,7 +209,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="6" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -219,583 +223,583 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
     </row>
-    <row r="76" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
     </row>
-    <row r="78" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
     </row>
-    <row r="79" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
     </row>
-    <row r="80" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
     </row>
-    <row r="81" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
     </row>
-    <row r="82" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
     </row>
-    <row r="83" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
     </row>
-    <row r="84" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
     </row>
-    <row r="86" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
     </row>
-    <row r="87" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
     </row>
-    <row r="99" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
     </row>
-    <row r="100" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" s="6" customFormat="true" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>

</xml_diff>